<commit_message>
adding remainder of 2025 data, updating analysis and data takeaways, revising index, and adding info about prisoner deaths
</commit_message>
<xml_diff>
--- a/data-original/2025_indoor/09.2025 - SB1R56.xlsx
+++ b/data-original/2025_indoor/09.2025 - SB1R56.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29303"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tdcj093.sharepoint.com/sites/CID P_O/Shared Documents/Rider 56/Rider 56 Reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilydemotte/MIG/tdcj-prison-heat/data-original/2025_indoor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{185DD93E-8EDA-4F96-94A7-BC80CA3A1E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF2BFCB-5718-EA4A-B215-ED17E0A32E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="1635" windowWidth="26190" windowHeight="14565" xr2:uid="{3D77639B-4A49-41E6-A0C4-589CF0897135}"/>
+    <workbookView xWindow="2600" yWindow="1640" windowWidth="26200" windowHeight="14560" xr2:uid="{3D77639B-4A49-41E6-A0C4-589CF0897135}"/>
   </bookViews>
   <sheets>
     <sheet name="SB1R56" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="74">
   <si>
     <t>September 2025</t>
   </si>
@@ -227,9 +227,6 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>81 .2</t>
-  </si>
-  <si>
     <t>Stevenson</t>
   </si>
   <si>
@@ -274,7 +271,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -739,23 +736,23 @@
   </sheetPr>
   <dimension ref="A1:AI69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1:AG2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="106" workbookViewId="0">
+      <selection activeCell="O58" sqref="O58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="12" width="6.140625" style="10" customWidth="1"/>
-    <col min="13" max="14" width="6.140625" style="14" customWidth="1"/>
-    <col min="15" max="31" width="6.140625" style="10" customWidth="1"/>
-    <col min="32" max="32" width="6.140625" style="10" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="18.7109375" style="12" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="6.1640625" style="10" customWidth="1"/>
+    <col min="13" max="14" width="6.1640625" style="14" customWidth="1"/>
+    <col min="15" max="31" width="6.1640625" style="10" customWidth="1"/>
+    <col min="32" max="32" width="6.1640625" style="10" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="18.6640625" style="12" hidden="1" customWidth="1"/>
     <col min="34" max="35" width="0" style="10" hidden="1" customWidth="1"/>
-    <col min="36" max="16384" width="9.140625" style="10" hidden="1"/>
+    <col min="36" max="16384" width="9.1640625" style="10" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="1" customFormat="1" ht="27.95" customHeight="1">
+    <row r="1" spans="1:35" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -794,7 +791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="5" customFormat="1">
+    <row r="2" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4">
         <v>1</v>
@@ -893,7 +890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -997,7 +994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -1096,7 +1093,7 @@
       </c>
       <c r="AI4" s="11"/>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -1197,7 +1194,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1298,7 +1295,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -1396,7 +1393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -1494,7 +1491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -1592,7 +1589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
@@ -1690,7 +1687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -1788,7 +1785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -1886,7 +1883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1984,7 +1981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
@@ -2082,7 +2079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -2180,7 +2177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
@@ -2278,7 +2275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>21</v>
       </c>
@@ -2376,7 +2373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>22</v>
       </c>
@@ -2474,7 +2471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>23</v>
       </c>
@@ -2572,7 +2569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
@@ -2670,7 +2667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>25</v>
       </c>
@@ -2768,7 +2765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>26</v>
       </c>
@@ -2866,7 +2863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>27</v>
       </c>
@@ -2964,7 +2961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:32">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
@@ -3062,7 +3059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>29</v>
       </c>
@@ -3160,7 +3157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:32">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
@@ -3258,7 +3255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:32">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
@@ -3356,7 +3353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:32">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>32</v>
       </c>
@@ -3454,7 +3451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:32">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>33</v>
       </c>
@@ -3552,7 +3549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:32">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>34</v>
       </c>
@@ -3650,7 +3647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:32">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>35</v>
       </c>
@@ -3748,7 +3745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:32">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>36</v>
       </c>
@@ -3846,7 +3843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:32">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>37</v>
       </c>
@@ -3944,7 +3941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:32">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>38</v>
       </c>
@@ -4042,7 +4039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:32">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>39</v>
       </c>
@@ -4140,7 +4137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:32">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>40</v>
       </c>
@@ -4238,7 +4235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:32">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>41</v>
       </c>
@@ -4336,7 +4333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:32">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>42</v>
       </c>
@@ -4434,7 +4431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:32">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>43</v>
       </c>
@@ -4532,7 +4529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:32">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>44</v>
       </c>
@@ -4630,7 +4627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:32">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>45</v>
       </c>
@@ -4728,7 +4725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:32">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>46</v>
       </c>
@@ -4826,7 +4823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:32">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>47</v>
       </c>
@@ -4924,7 +4921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:32">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>48</v>
       </c>
@@ -5022,7 +5019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:32">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>49</v>
       </c>
@@ -5120,7 +5117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:32">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>50</v>
       </c>
@@ -5218,7 +5215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:32">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>51</v>
       </c>
@@ -5316,7 +5313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:32">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>52</v>
       </c>
@@ -5414,7 +5411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:32">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>53</v>
       </c>
@@ -5512,7 +5509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:32">
+    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>54</v>
       </c>
@@ -5610,7 +5607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:32">
+    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>55</v>
       </c>
@@ -5708,7 +5705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:32">
+    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>56</v>
       </c>
@@ -5806,7 +5803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:32">
+    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>57</v>
       </c>
@@ -5904,7 +5901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:32">
+    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>58</v>
       </c>
@@ -6002,7 +5999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:32">
+    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>59</v>
       </c>
@@ -6100,7 +6097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:32">
+    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>60</v>
       </c>
@@ -6198,7 +6195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:32">
+    <row r="57" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>61</v>
       </c>
@@ -6241,8 +6238,8 @@
       <c r="N57" s="8">
         <v>82.8</v>
       </c>
-      <c r="O57" s="8" t="s">
-        <v>62</v>
+      <c r="O57" s="8">
+        <v>81.2</v>
       </c>
       <c r="P57" s="8">
         <v>82.4</v>
@@ -6296,9 +6293,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:32">
+    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58" s="8">
         <v>89.9</v>
@@ -6394,9 +6391,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:32">
+    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" s="8">
         <v>85.3</v>
@@ -6492,9 +6489,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:32">
+    <row r="60" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" s="8">
         <v>84.2</v>
@@ -6590,9 +6587,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:32">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61" s="8">
         <v>84.2</v>
@@ -6688,9 +6685,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:32">
+    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B62" s="8">
         <v>87.1</v>
@@ -6786,9 +6783,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:32">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B63" s="8">
         <v>87.1</v>
@@ -6884,9 +6881,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:32">
+    <row r="64" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B64" s="8">
         <v>87.3</v>
@@ -6982,9 +6979,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:32">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B65" s="8">
         <v>85.6</v>
@@ -7080,9 +7077,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:32">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B66" s="8">
         <v>87.8</v>
@@ -7178,9 +7175,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:32">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B67" s="8">
         <v>86</v>
@@ -7276,9 +7273,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:32">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B68" s="8">
         <v>86.9</v>
@@ -7374,9 +7371,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:32">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B69" s="8">
         <v>87</v>
@@ -7485,38 +7482,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b68152e1-1881-4013-b170-313eae0e7cc6" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="db7a3a59-73db-48d9-8748-b4b5426a67ab">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Number xmlns="db7a3a59-73db-48d9-8748-b4b5426a67ab" xsi:nil="true"/>
-    <DateTime xmlns="db7a3a59-73db-48d9-8748-b4b5426a67ab" xsi:nil="true"/>
-    <SharedWithUsers xmlns="b68152e1-1881-4013-b170-313eae0e7cc6">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="db7a3a59-73db-48d9-8748-b4b5426a67ab" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AD904CCEBA22F8488B5CEC69CF303386" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f66fa6ed6f9328ffce6efb00a1b8e295">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="db7a3a59-73db-48d9-8748-b4b5426a67ab" xmlns:ns3="b68152e1-1881-4013-b170-313eae0e7cc6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c077d5b373feffbbad9cda7228bd648" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7800,14 +7765,74 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b68152e1-1881-4013-b170-313eae0e7cc6" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="db7a3a59-73db-48d9-8748-b4b5426a67ab">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Number xmlns="db7a3a59-73db-48d9-8748-b4b5426a67ab" xsi:nil="true"/>
+    <DateTime xmlns="db7a3a59-73db-48d9-8748-b4b5426a67ab" xsi:nil="true"/>
+    <SharedWithUsers xmlns="b68152e1-1881-4013-b170-313eae0e7cc6">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="db7a3a59-73db-48d9-8748-b4b5426a67ab" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC6779AB-9CD6-4E99-8472-E76547FE1B6D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B655EBFA-A52A-4D77-A713-46F8836181AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="db7a3a59-73db-48d9-8748-b4b5426a67ab"/>
+    <ds:schemaRef ds:uri="b68152e1-1881-4013-b170-313eae0e7cc6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05E760D-501D-4982-A08E-044CF45170D1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05E760D-501D-4982-A08E-044CF45170D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B655EBFA-A52A-4D77-A713-46F8836181AC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC6779AB-9CD6-4E99-8472-E76547FE1B6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b68152e1-1881-4013-b170-313eae0e7cc6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="db7a3a59-73db-48d9-8748-b4b5426a67ab"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>